<commit_message>
Added game client overview
</commit_message>
<xml_diff>
--- a/Anniv.xlsx
+++ b/Anniv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CTables\Wartune\Wartune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1844DFBA-3A0F-4EA1-9AA7-AE9276A070B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44DF84F-F465-4632-86F3-588F39814CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19318" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -709,14 +709,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -734,6 +737,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -757,33 +769,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1147,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6400203-2BDE-4802-8A79-E79C2E94A689}">
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1158,43 +1148,43 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="2:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="2:10" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="33"/>
@@ -1221,43 +1211,43 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="2:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="2:10" ht="4.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
@@ -1271,56 +1261,56 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
     </row>
     <row r="15" spans="2:10" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="34"/>
@@ -1334,56 +1324,56 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="50"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="2:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
@@ -1443,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1463,11 +1453,11 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
       <c r="H1" s="23" t="s">
         <v>105</v>
       </c>
@@ -1857,14 +1847,14 @@
         <v>1</v>
       </c>
       <c r="E26" s="11">
-        <f>C26*D26</f>
+        <f t="shared" ref="E26:E51" si="0">C26*D26</f>
         <v>1</v>
       </c>
       <c r="F26" s="7">
         <v>100</v>
       </c>
       <c r="G26" s="7">
-        <f>C26*F26</f>
+        <f t="shared" ref="G26:G51" si="1">C26*F26</f>
         <v>100</v>
       </c>
     </row>
@@ -1879,14 +1869,14 @@
         <v>1</v>
       </c>
       <c r="E27" s="18">
-        <f>C27*D27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F27" s="17">
         <v>100</v>
       </c>
       <c r="G27" s="17">
-        <f>C27*F27</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1901,14 +1891,14 @@
         <v>20</v>
       </c>
       <c r="E28" s="11">
-        <f>C28*D28</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
       </c>
       <c r="G28" s="7">
-        <f>C28*F28</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
     </row>
@@ -1923,14 +1913,14 @@
         <v>40</v>
       </c>
       <c r="E29" s="11">
-        <f>C29*D29</f>
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <f>C29*F29</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
     </row>
@@ -1945,14 +1935,14 @@
         <v>20</v>
       </c>
       <c r="E30" s="11">
-        <f>C30*D30</f>
+        <f t="shared" si="0"/>
         <v>25000</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="7">
-        <f>C30*F30</f>
+        <f t="shared" si="1"/>
         <v>1250</v>
       </c>
     </row>
@@ -1967,14 +1957,14 @@
         <v>20</v>
       </c>
       <c r="E31" s="11">
-        <f>C31*D31</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="7">
-        <f>C31*F31</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
@@ -1989,14 +1979,14 @@
         <v>20</v>
       </c>
       <c r="E32" s="11">
-        <f>C32*D32</f>
+        <f t="shared" si="0"/>
         <v>40000</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="G32" s="7">
-        <f>C32*F32</f>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
     </row>
@@ -2011,14 +2001,14 @@
         <v>10</v>
       </c>
       <c r="E33" s="11">
-        <f>C33*D33</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="7">
-        <f>C33*F33</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2033,14 +2023,14 @@
         <v>4</v>
       </c>
       <c r="E34" s="11">
-        <f>C34*D34</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
       <c r="G34" s="7">
-        <f>C34*F34</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2055,14 +2045,14 @@
         <v>4</v>
       </c>
       <c r="E35" s="18">
-        <f>C35*D35</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F35" s="17">
         <v>5</v>
       </c>
       <c r="G35" s="17">
-        <f>C35*F35</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2077,14 +2067,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="11">
-        <f>C36*D36</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F36" s="7">
         <v>5</v>
       </c>
       <c r="G36" s="7">
-        <f>C36*F36</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2099,14 +2089,14 @@
         <v>2</v>
       </c>
       <c r="E37" s="18">
-        <f>C37*D37</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F37" s="17">
         <v>25</v>
       </c>
       <c r="G37" s="17">
-        <f>C37*F37</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -2121,14 +2111,14 @@
         <v>2</v>
       </c>
       <c r="E38" s="18">
-        <f>C38*D38</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F38" s="17">
         <v>5</v>
       </c>
       <c r="G38" s="17">
-        <f>C38*F38</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
     </row>
@@ -2143,14 +2133,14 @@
         <v>4</v>
       </c>
       <c r="E39" s="18">
-        <f>C39*D39</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F39" s="17">
         <v>5</v>
       </c>
       <c r="G39" s="17">
-        <f>C39*F39</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2165,14 +2155,14 @@
         <v>1</v>
       </c>
       <c r="E40" s="11">
-        <f>C40*D40</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F40" s="7">
         <v>5</v>
       </c>
       <c r="G40" s="7">
-        <f>C40*F40</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2187,14 +2177,14 @@
         <v>1</v>
       </c>
       <c r="E41" s="18">
-        <f>C41*D41</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F41" s="17">
         <v>7</v>
       </c>
       <c r="G41" s="17">
-        <f>C41*F41</f>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
     </row>
@@ -2209,14 +2199,14 @@
         <v>1</v>
       </c>
       <c r="E42" s="18">
-        <f>C42*D42</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F42" s="17">
         <v>10</v>
       </c>
       <c r="G42" s="17">
-        <f>C42*F42</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2231,14 +2221,14 @@
         <v>2</v>
       </c>
       <c r="E43" s="11">
-        <f>C43*D43</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F43" s="7">
         <v>2</v>
       </c>
       <c r="G43" s="7">
-        <f>C43*F43</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2253,14 +2243,14 @@
         <v>2</v>
       </c>
       <c r="E44" s="18">
-        <f>C44*D44</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F44" s="17">
         <v>200</v>
       </c>
       <c r="G44" s="17">
-        <f>C44*F44</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -2275,14 +2265,14 @@
         <v>1</v>
       </c>
       <c r="E45" s="18">
-        <f>C45*D45</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F45" s="17">
         <v>20</v>
       </c>
       <c r="G45" s="17">
-        <f>C45*F45</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -2297,14 +2287,14 @@
         <v>1</v>
       </c>
       <c r="E46" s="18">
-        <f>C46*D46</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F46" s="17">
         <v>30</v>
       </c>
       <c r="G46" s="17">
-        <f>C46*F46</f>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
     </row>
@@ -2319,14 +2309,14 @@
         <v>1</v>
       </c>
       <c r="E47" s="18">
-        <f>C47*D47</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F47" s="17">
         <v>40</v>
       </c>
       <c r="G47" s="17">
-        <f>C47*F47</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
@@ -2341,14 +2331,14 @@
         <v>1</v>
       </c>
       <c r="E48" s="18">
-        <f>C48*D48</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F48" s="17">
         <v>50</v>
       </c>
       <c r="G48" s="17">
-        <f>C48*F48</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -2363,14 +2353,14 @@
         <v>1</v>
       </c>
       <c r="E49" s="18">
-        <f>C49*D49</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F49" s="17">
         <v>1</v>
       </c>
       <c r="G49" s="17">
-        <f>C49*F49</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2385,14 +2375,14 @@
         <v>1</v>
       </c>
       <c r="E50" s="18">
-        <f>C50*D50</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F50" s="17">
         <v>1</v>
       </c>
       <c r="G50" s="17">
-        <f>C50*F50</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2407,14 +2397,14 @@
         <v>1</v>
       </c>
       <c r="E51" s="21">
-        <f>C51*D51</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F51" s="20">
         <v>1</v>
       </c>
       <c r="G51" s="20">
-        <f>C51*F51</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2449,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A099BD42-EDC1-43FC-957F-85D4BF1921DE}">
   <dimension ref="B1:J78"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74:G74"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2469,11 +2459,11 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
       <c r="I1" s="23" t="s">
         <v>105</v>
       </c>
@@ -2830,10 +2820,10 @@
       <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="47"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
@@ -2845,10 +2835,10 @@
       <c r="D19" s="11">
         <v>10</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="47"/>
+      <c r="J19" s="51"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
@@ -2860,10 +2850,10 @@
       <c r="D20" s="11">
         <v>15</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="I20" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="J20" s="47"/>
+      <c r="J20" s="51"/>
     </row>
     <row r="21" spans="2:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
@@ -2875,10 +2865,10 @@
       <c r="D21" s="14">
         <v>25</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="J21" s="47"/>
+      <c r="J21" s="51"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -2888,10 +2878,10 @@
         <f>14*60</f>
         <v>840</v>
       </c>
-      <c r="I22" s="53" t="s">
+      <c r="I22" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="47"/>
+      <c r="J22" s="51"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="32" t="s">
@@ -2937,17 +2927,17 @@
         <v>1</v>
       </c>
       <c r="E26" s="11">
-        <f>C26*D26</f>
+        <f t="shared" ref="E26:E72" si="0">C26*D26</f>
         <v>1</v>
       </c>
       <c r="F26" s="7">
         <v>100</v>
       </c>
       <c r="G26" s="7">
-        <f>C26*F26</f>
+        <f t="shared" ref="G26:G72" si="1">C26*F26</f>
         <v>100</v>
       </c>
-      <c r="H26" s="54">
+      <c r="H26" s="38">
         <v>1</v>
       </c>
     </row>
@@ -2962,17 +2952,17 @@
         <v>1</v>
       </c>
       <c r="E27" s="18">
-        <f>C27*D27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F27" s="17">
         <v>100</v>
       </c>
       <c r="G27" s="17">
-        <f>C27*F27</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H27" s="55">
+      <c r="H27" s="39">
         <v>0</v>
       </c>
     </row>
@@ -2987,17 +2977,17 @@
         <v>20</v>
       </c>
       <c r="E28" s="11">
-        <f>C28*D28</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
       </c>
       <c r="G28" s="7">
-        <f>C28*F28</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H28" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3012,17 +3002,17 @@
         <v>20</v>
       </c>
       <c r="E29" s="11">
-        <f>C29*D29</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <f>C29*F29</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H29" s="54">
+      <c r="H29" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3037,17 +3027,17 @@
         <v>20</v>
       </c>
       <c r="E30" s="11">
-        <f>C30*D30</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="7">
-        <f>C30*F30</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3062,17 +3052,17 @@
         <v>10</v>
       </c>
       <c r="E31" s="11">
-        <f>C31*D31</f>
+        <f t="shared" si="0"/>
         <v>25000</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="7">
-        <f>C31*F31</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3087,17 +3077,17 @@
         <v>10</v>
       </c>
       <c r="E32" s="11">
-        <f>C32*D32</f>
+        <f t="shared" si="0"/>
         <v>25000</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="G32" s="7">
-        <f>C32*F32</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H32" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3112,17 +3102,17 @@
         <v>20</v>
       </c>
       <c r="E33" s="18">
-        <f>C33*D33</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F33" s="17">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <f>C33*F33</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H33" s="55">
+      <c r="H33" s="39">
         <v>1</v>
       </c>
     </row>
@@ -3137,17 +3127,17 @@
         <v>2</v>
       </c>
       <c r="E34" s="11">
-        <f>C34*D34</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
       <c r="G34" s="7">
-        <f>C34*F34</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H34" s="54">
+      <c r="H34" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3162,17 +3152,17 @@
         <v>6</v>
       </c>
       <c r="E35" s="11">
-        <f>C35*D35</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F35" s="7">
         <v>1</v>
       </c>
       <c r="G35" s="7">
-        <f>C35*F35</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3187,17 +3177,17 @@
         <v>6</v>
       </c>
       <c r="E36" s="11">
-        <f>C36*D36</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
       <c r="G36" s="7">
-        <f>C36*F36</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H36" s="54">
+      <c r="H36" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3212,17 +3202,17 @@
         <v>20</v>
       </c>
       <c r="E37" s="11">
-        <f>C37*D37</f>
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
       <c r="G37" s="7">
-        <f>C37*F37</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H37" s="54">
+      <c r="H37" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3237,17 +3227,17 @@
         <v>40</v>
       </c>
       <c r="E38" s="11">
-        <f>C38*D38</f>
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
       <c r="G38" s="7">
-        <f>C38*F38</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="H38" s="54">
+      <c r="H38" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3262,17 +3252,17 @@
         <v>20</v>
       </c>
       <c r="E39" s="11">
-        <f>C39*D39</f>
+        <f t="shared" si="0"/>
         <v>25000</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="7">
-        <f>C39*F39</f>
+        <f t="shared" si="1"/>
         <v>1250</v>
       </c>
-      <c r="H39" s="54">
+      <c r="H39" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3287,17 +3277,17 @@
         <v>20</v>
       </c>
       <c r="E40" s="11">
-        <f>C40*D40</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
       </c>
       <c r="G40" s="7">
-        <f>C40*F40</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="H40" s="54">
+      <c r="H40" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3312,17 +3302,17 @@
         <v>20</v>
       </c>
       <c r="E41" s="11">
-        <f>C41*D41</f>
+        <f t="shared" si="0"/>
         <v>40000</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
       </c>
       <c r="G41" s="7">
-        <f>C41*F41</f>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="H41" s="54">
+      <c r="H41" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3337,17 +3327,17 @@
         <v>10</v>
       </c>
       <c r="E42" s="11">
-        <f>C42*D42</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="F42" s="7">
         <v>1</v>
       </c>
       <c r="G42" s="7">
-        <f>C42*F42</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H42" s="54">
+      <c r="H42" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3362,17 +3352,17 @@
         <v>4</v>
       </c>
       <c r="E43" s="18">
-        <f>C43*D43</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F43" s="17">
         <v>1</v>
       </c>
       <c r="G43" s="17">
-        <f>C43*F43</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H43" s="55">
+      <c r="H43" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3387,17 +3377,17 @@
         <v>4</v>
       </c>
       <c r="E44" s="18">
-        <f>C44*D44</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F44" s="17">
         <v>5</v>
       </c>
       <c r="G44" s="17">
-        <f>C44*F44</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H44" s="55">
+      <c r="H44" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3412,17 +3402,17 @@
         <v>2</v>
       </c>
       <c r="E45" s="11">
-        <f>C45*D45</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F45" s="7">
         <v>5</v>
       </c>
       <c r="G45" s="7">
-        <f>C45*F45</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H45" s="54">
+      <c r="H45" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3437,17 +3427,17 @@
         <v>2</v>
       </c>
       <c r="E46" s="18">
-        <f>C46*D46</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F46" s="17">
         <v>25</v>
       </c>
       <c r="G46" s="17">
-        <f>C46*F46</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="H46" s="55">
+      <c r="H46" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3462,17 +3452,17 @@
         <v>2</v>
       </c>
       <c r="E47" s="18">
-        <f>C47*D47</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F47" s="17">
         <v>5</v>
       </c>
       <c r="G47" s="17">
-        <f>C47*F47</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="H47" s="55">
+      <c r="H47" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3487,17 +3477,17 @@
         <v>4</v>
       </c>
       <c r="E48" s="18">
-        <f>C48*D48</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F48" s="17">
         <v>5</v>
       </c>
       <c r="G48" s="17">
-        <f>C48*F48</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H48" s="55">
+      <c r="H48" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3512,17 +3502,17 @@
         <v>1</v>
       </c>
       <c r="E49" s="18">
-        <f>C49*D49</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F49" s="17">
         <v>5</v>
       </c>
       <c r="G49" s="17">
-        <f>C49*F49</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H49" s="55">
+      <c r="H49" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3537,17 +3527,17 @@
         <v>1</v>
       </c>
       <c r="E50" s="18">
-        <f>C50*D50</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F50" s="17">
         <v>7</v>
       </c>
       <c r="G50" s="17">
-        <f>C50*F50</f>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
-      <c r="H50" s="55">
+      <c r="H50" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3562,17 +3552,17 @@
         <v>1</v>
       </c>
       <c r="E51" s="18">
-        <f>C51*D51</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F51" s="17">
         <v>10</v>
       </c>
       <c r="G51" s="17">
-        <f>C51*F51</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H51" s="55">
+      <c r="H51" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3587,17 +3577,17 @@
         <v>3</v>
       </c>
       <c r="E52" s="11">
-        <f>C52*D52</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F52" s="7">
         <v>1</v>
       </c>
       <c r="G52" s="7">
-        <f>C52*F52</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H52" s="56">
+      <c r="H52" s="40">
         <v>1</v>
       </c>
     </row>
@@ -3612,17 +3602,17 @@
         <v>3</v>
       </c>
       <c r="E53" s="11">
-        <f>C53*D53</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
       <c r="G53" s="7">
-        <f>C53*F53</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H53" s="54">
+      <c r="H53" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3637,17 +3627,17 @@
         <v>3</v>
       </c>
       <c r="E54" s="11">
-        <f>C54*D54</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F54" s="7">
         <v>1</v>
       </c>
       <c r="G54" s="7">
-        <f>C54*F54</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H54" s="54">
+      <c r="H54" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3662,17 +3652,17 @@
         <v>3</v>
       </c>
       <c r="E55" s="11">
-        <f>C55*D55</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="F55" s="7">
         <v>1</v>
       </c>
       <c r="G55" s="7">
-        <f>C55*F55</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H55" s="54">
+      <c r="H55" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3687,17 +3677,17 @@
         <v>10</v>
       </c>
       <c r="E56" s="11">
-        <f>C56*D56</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="F56" s="7">
         <v>1</v>
       </c>
       <c r="G56" s="7">
-        <f>C56*F56</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H56" s="54">
+      <c r="H56" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3712,17 +3702,17 @@
         <v>4</v>
       </c>
       <c r="E57" s="11">
-        <f>C57*D57</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="F57" s="7">
         <v>1</v>
       </c>
       <c r="G57" s="7">
-        <f>C57*F57</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H57" s="54">
+      <c r="H57" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3737,17 +3727,17 @@
         <v>6</v>
       </c>
       <c r="E58" s="11">
-        <f>C58*D58</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="F58" s="7">
         <v>1</v>
       </c>
       <c r="G58" s="7">
-        <f>C58*F58</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H58" s="54">
+      <c r="H58" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3762,17 +3752,17 @@
         <v>2</v>
       </c>
       <c r="E59" s="18">
-        <f>C59*D59</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F59" s="17">
         <v>5</v>
       </c>
       <c r="G59" s="17">
-        <f>C59*F59</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="H59" s="55">
+      <c r="H59" s="39">
         <v>1</v>
       </c>
     </row>
@@ -3787,17 +3777,17 @@
         <v>1</v>
       </c>
       <c r="E60" s="18">
-        <f>C60*D60</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F60" s="17">
         <v>1</v>
       </c>
       <c r="G60" s="17">
-        <f>C60*F60</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H60" s="55">
+      <c r="H60" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3812,17 +3802,17 @@
         <v>1</v>
       </c>
       <c r="E61" s="18">
-        <f>C61*D61</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F61" s="17">
         <v>1</v>
       </c>
       <c r="G61" s="17">
-        <f>C61*F61</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H61" s="55">
+      <c r="H61" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3837,17 +3827,17 @@
         <v>1</v>
       </c>
       <c r="E62" s="18">
-        <f>C62*D62</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F62" s="17">
         <v>1</v>
       </c>
       <c r="G62" s="17">
-        <f>C62*F62</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H62" s="55">
+      <c r="H62" s="39">
         <v>0</v>
       </c>
     </row>
@@ -3862,17 +3852,17 @@
         <v>4</v>
       </c>
       <c r="E63" s="11">
-        <f>C63*D63</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="F63" s="7">
         <v>1</v>
       </c>
       <c r="G63" s="7">
-        <f>C63*F63</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H63" s="54">
+      <c r="H63" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3887,17 +3877,17 @@
         <v>2</v>
       </c>
       <c r="E64" s="11">
-        <f>C64*D64</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F64" s="7">
         <v>2</v>
       </c>
       <c r="G64" s="7">
-        <f>C64*F64</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H64" s="54">
+      <c r="H64" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3912,17 +3902,17 @@
         <v>2</v>
       </c>
       <c r="E65" s="11">
-        <f>C65*D65</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F65" s="7">
         <v>200</v>
       </c>
       <c r="G65" s="7">
-        <f>C65*F65</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="H65" s="54">
+      <c r="H65" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3937,17 +3927,17 @@
         <v>1</v>
       </c>
       <c r="E66" s="11">
-        <f>C66*D66</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F66" s="7">
         <v>20</v>
       </c>
       <c r="G66" s="7">
-        <f>C66*F66</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H66" s="54">
+      <c r="H66" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3962,17 +3952,17 @@
         <v>5</v>
       </c>
       <c r="E67" s="11">
-        <f>C67*D67</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F67" s="7">
         <v>1</v>
       </c>
       <c r="G67" s="7">
-        <f>C67*F67</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="H67" s="54">
+      <c r="H67" s="38">
         <v>1</v>
       </c>
     </row>
@@ -3987,17 +3977,17 @@
         <v>4</v>
       </c>
       <c r="E68" s="18">
-        <f>C68*D68</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="F68" s="17">
         <v>1</v>
       </c>
       <c r="G68" s="17">
-        <f>C68*F68</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H68" s="55">
+      <c r="H68" s="39">
         <v>1</v>
       </c>
     </row>
@@ -4012,17 +4002,17 @@
         <v>4</v>
       </c>
       <c r="E69" s="18">
-        <f>C69*D69</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="F69" s="17">
         <v>1</v>
       </c>
       <c r="G69" s="17">
-        <f>C69*F69</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H69" s="55">
+      <c r="H69" s="39">
         <v>1</v>
       </c>
     </row>
@@ -4037,17 +4027,17 @@
         <v>1</v>
       </c>
       <c r="E70" s="11">
-        <f>C70*D70</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F70" s="7">
         <v>15</v>
       </c>
       <c r="G70" s="7">
-        <f>C70*F70</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="H70" s="54">
+      <c r="H70" s="38">
         <v>1</v>
       </c>
     </row>
@@ -4062,17 +4052,17 @@
         <v>1</v>
       </c>
       <c r="E71" s="18">
-        <f>C71*D71</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F71" s="17">
         <v>20</v>
       </c>
       <c r="G71" s="17">
-        <f>C71*F71</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H71" s="55">
+      <c r="H71" s="39">
         <v>1</v>
       </c>
     </row>
@@ -4087,17 +4077,17 @@
         <v>1</v>
       </c>
       <c r="E72" s="21">
-        <f>C72*D72</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F72" s="20">
         <v>25</v>
       </c>
       <c r="G72" s="20">
-        <f>C72*F72</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="H72" s="57">
+      <c r="H72" s="41">
         <v>1</v>
       </c>
     </row>
@@ -4157,10 +4147,10 @@
     <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="H26:H72">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>